<commit_message>
last commit before downloading readme
</commit_message>
<xml_diff>
--- a/data/mine_attributes.xlsx
+++ b/data/mine_attributes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/Documents/University Work/summer internship/pycharm_factory/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/Documents/University Work/summer internship/FUSE/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12342810-4D73-804B-9CAF-03EA626C03AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F0590FC-DB72-5745-92E8-4581E7388B58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35580" yWindow="-900" windowWidth="28040" windowHeight="16940" xr2:uid="{E883CBF3-2CDB-0D4C-B75C-CDFD4FA8C312}"/>
+    <workbookView xWindow="30140" yWindow="-640" windowWidth="28040" windowHeight="16940" activeTab="8" xr2:uid="{E883CBF3-2CDB-0D4C-B75C-CDFD4FA8C312}"/>
   </bookViews>
   <sheets>
     <sheet name="macro details" sheetId="8" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <sheet name="worker" sheetId="9" r:id="rId10"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="64">
   <si>
     <t xml:space="preserve">company </t>
   </si>
@@ -233,6 +233,9 @@
   </si>
   <si>
     <t>st</t>
+  </si>
+  <si>
+    <t>hr/wk</t>
   </si>
 </sst>
 </file>
@@ -589,7 +592,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ABFB296-438E-1747-ABC9-555CDE54E2A4}">
   <dimension ref="A2:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -874,7 +877,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -967,9 +970,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62385A2F-9BCF-E84D-987B-70F09662E5AB}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1051,7 +1052,7 @@
   <dimension ref="A2:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1085,6 +1086,9 @@
       <c r="B4">
         <v>110</v>
       </c>
+      <c r="C4" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -1092,6 +1096,9 @@
       </c>
       <c r="B5">
         <v>60</v>
+      </c>
+      <c r="C5" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1168,7 +1175,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C99E2633-F0B0-0F4F-8FA5-326C9D7CE73B}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
implemented room and pillar method with all the qMachines
</commit_message>
<xml_diff>
--- a/data/mine_attributes.xlsx
+++ b/data/mine_attributes.xlsx
@@ -1,29 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/Documents/University Work/summer internship/FUSE/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F0590FC-DB72-5745-92E8-4581E7388B58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9E310BF-2B7D-AC44-9EC4-4063C47D3817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30140" yWindow="-640" windowWidth="28040" windowHeight="16940" activeTab="8" xr2:uid="{E883CBF3-2CDB-0D4C-B75C-CDFD4FA8C312}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{E883CBF3-2CDB-0D4C-B75C-CDFD4FA8C312}"/>
   </bookViews>
   <sheets>
     <sheet name="macro details" sheetId="8" r:id="rId1"/>
     <sheet name="utility" sheetId="10" r:id="rId2"/>
-    <sheet name="continuous miner" sheetId="4" r:id="rId3"/>
-    <sheet name="roof bolter" sheetId="6" r:id="rId4"/>
-    <sheet name="longwall shearer" sheetId="11" r:id="rId5"/>
-    <sheet name="AFC" sheetId="13" r:id="rId6"/>
-    <sheet name="stage loader" sheetId="14" r:id="rId7"/>
-    <sheet name="LHD" sheetId="12" r:id="rId8"/>
-    <sheet name="shuttle car" sheetId="5" r:id="rId9"/>
-    <sheet name="worker" sheetId="9" r:id="rId10"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId11"/>
+    <sheet name="r &amp; p method" sheetId="15" r:id="rId3"/>
+    <sheet name="continuous miner" sheetId="4" r:id="rId4"/>
+    <sheet name="roof bolter" sheetId="6" r:id="rId5"/>
+    <sheet name="longwall shearer" sheetId="11" r:id="rId6"/>
+    <sheet name="AFC" sheetId="13" r:id="rId7"/>
+    <sheet name="stage loader" sheetId="14" r:id="rId8"/>
+    <sheet name="LHD" sheetId="12" r:id="rId9"/>
+    <sheet name="shuttle car" sheetId="5" r:id="rId10"/>
+    <sheet name="worker" sheetId="9" r:id="rId11"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="66">
   <si>
     <t xml:space="preserve">company </t>
   </si>
@@ -172,9 +173,6 @@
     <t>Green River, WY</t>
   </si>
   <si>
-    <t xml:space="preserve">value </t>
-  </si>
-  <si>
     <t>unit</t>
   </si>
   <si>
@@ -205,18 +203,9 @@
     <t>g/cm3</t>
   </si>
   <si>
-    <t>hrs/wk</t>
-  </si>
-  <si>
-    <t>usage</t>
-  </si>
-  <si>
     <t>production output</t>
   </si>
   <si>
-    <t>maintenance</t>
-  </si>
-  <si>
     <t>workers</t>
   </si>
   <si>
@@ -232,20 +221,45 @@
     <t>7LS5</t>
   </si>
   <si>
-    <t>st</t>
-  </si>
-  <si>
-    <t>hr/wk</t>
+    <t>shuttle car</t>
+  </si>
+  <si>
+    <t>LHD</t>
+  </si>
+  <si>
+    <t>worker</t>
+  </si>
+  <si>
+    <t>mining operating</t>
+  </si>
+  <si>
+    <t>period</t>
+  </si>
+  <si>
+    <t>maintenance operating</t>
+  </si>
+  <si>
+    <t>non operating</t>
+  </si>
+  <si>
+    <t>MADEUP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -271,11 +285,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -590,10 +605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ABFB296-438E-1747-ABC9-555CDE54E2A4}">
-  <dimension ref="A2:C9"/>
+  <dimension ref="A2:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -626,13 +641,13 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B4">
         <v>475</v>
       </c>
       <c r="C4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -659,13 +674,13 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B7">
         <v>2.13</v>
       </c>
       <c r="C7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -678,13 +693,58 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B9">
         <v>250</v>
       </c>
       <c r="C9" t="s">
-        <v>47</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10">
+        <v>250</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11">
+        <f>B13-B10</f>
+        <v>115</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="2">
+        <v>365</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -694,11 +754,84 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C99E2633-F0B0-0F4F-8FA5-326C9D7CE73B}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="27" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4">
+        <v>85</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA6ED9ED-AFC7-5E4D-A019-3E513DE76C3A}">
   <dimension ref="A2:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -708,26 +841,26 @@
         <v>20</v>
       </c>
       <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
         <v>42</v>
-      </c>
-      <c r="C2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3">
         <v>70000</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B4">
         <v>10</v>
@@ -741,7 +874,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{318DF2EB-565B-D749-9801-BCC60DA85E15}">
   <dimension ref="B2:I6"/>
   <sheetViews>
@@ -854,17 +987,17 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -873,11 +1006,74 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{635D5B4B-AA0D-8346-A63A-AAC97E12BBE4}">
+  <dimension ref="A2:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F6C306B-8A58-6F47-B920-204089AE08B3}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A3" sqref="A3:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -903,62 +1099,40 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" t="s">
-        <v>32</v>
+        <v>52</v>
+      </c>
+      <c r="B3">
+        <v>139</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="B4">
-        <v>139</v>
+        <v>600</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B5">
-        <v>110</v>
-      </c>
-      <c r="C5" t="s">
-        <v>53</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B6">
-        <v>60</v>
-      </c>
-      <c r="C6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7">
-        <v>600</v>
-      </c>
-      <c r="C7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>57</v>
-      </c>
-      <c r="B8">
-        <v>2</v>
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -966,11 +1140,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62385A2F-9BCF-E84D-987B-70F09662E5AB}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -995,51 +1171,29 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" t="s">
-        <v>33</v>
+        <v>31</v>
+      </c>
+      <c r="B3">
+        <v>125</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4">
-        <v>110</v>
-      </c>
-      <c r="C4" t="s">
-        <v>53</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B5">
-        <v>60</v>
-      </c>
-      <c r="C5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6">
-        <v>125</v>
-      </c>
-      <c r="C6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>57</v>
-      </c>
-      <c r="B7">
-        <v>3</v>
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1047,12 +1201,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6659977-9172-CD46-8451-C5DE37D17549}">
-  <dimension ref="A2:C7"/>
+  <dimension ref="A2:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A4" sqref="A4:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1065,12 +1219,12 @@
         <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B3">
         <v>900</v>
@@ -1081,34 +1235,12 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B4">
-        <v>110</v>
-      </c>
-      <c r="C4" t="s">
-        <v>63</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B5">
-        <v>60</v>
-      </c>
-      <c r="C5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1116,7 +1248,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D375DA5D-47B4-034B-A28D-715AAE1B79FC}">
   <dimension ref="A2:B2"/>
   <sheetViews>
@@ -1139,56 +1271,31 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20386E3A-C567-1F42-9477-9B986FE1CE0F}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{231CCEC4-3D3D-4143-AE0F-E82354A19379}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C99E2633-F0B0-0F4F-8FA5-326C9D7CE73B}">
-  <dimension ref="A1:C8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{231CCEC4-3D3D-4143-AE0F-E82354A19379}">
+  <dimension ref="A2:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27" customWidth="1"/>
+    <col min="1" max="1" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>25</v>
-      </c>
-    </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>20</v>
@@ -1197,67 +1304,45 @@
         <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B4">
-        <v>14</v>
+        <v>85</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B5">
-        <v>110</v>
-      </c>
-      <c r="C5" t="s">
-        <v>53</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B6">
-        <v>60</v>
-      </c>
-      <c r="C6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7">
-        <v>85</v>
-      </c>
-      <c r="C7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>57</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refined the methods removed arguments and added an opex
</commit_message>
<xml_diff>
--- a/data/mine_attributes.xlsx
+++ b/data/mine_attributes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/Documents/University Work/summer internship/FUSE/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01717EDE-67DC-BD41-AB25-E2ABB6068BF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6074664C-3846-964D-A303-777AC02383A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-3600" windowWidth="11040" windowHeight="21600" activeTab="3" xr2:uid="{E883CBF3-2CDB-0D4C-B75C-CDFD4FA8C312}"/>
+    <workbookView xWindow="100" yWindow="500" windowWidth="21560" windowHeight="17500" xr2:uid="{E883CBF3-2CDB-0D4C-B75C-CDFD4FA8C312}"/>
   </bookViews>
   <sheets>
     <sheet name="macro details" sheetId="8" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="78">
   <si>
     <t xml:space="preserve">company </t>
   </si>
@@ -156,9 +156,6 @@
     <t>ore grade</t>
   </si>
   <si>
-    <t>%</t>
-  </si>
-  <si>
     <t>mine operating production</t>
   </si>
   <si>
@@ -192,12 +189,6 @@
     <t>water</t>
   </si>
   <si>
-    <t>fuel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">electricity </t>
-  </si>
-  <si>
     <t>ore density</t>
   </si>
   <si>
@@ -250,6 +241,45 @@
   </si>
   <si>
     <t>longwall shearer</t>
+  </si>
+  <si>
+    <t>conversion efficiency</t>
+  </si>
+  <si>
+    <t>%/100</t>
+  </si>
+  <si>
+    <t>t shield</t>
+  </si>
+  <si>
+    <t>afc</t>
+  </si>
+  <si>
+    <t>flat link chain</t>
+  </si>
+  <si>
+    <t>low profile chain</t>
+  </si>
+  <si>
+    <t>afc drive</t>
+  </si>
+  <si>
+    <t>stage loader</t>
+  </si>
+  <si>
+    <t>borer miner</t>
+  </si>
+  <si>
+    <t>joy AFC</t>
+  </si>
+  <si>
+    <t>£/kWh</t>
+  </si>
+  <si>
+    <t>£/L</t>
+  </si>
+  <si>
+    <t>electricity</t>
   </si>
 </sst>
 </file>
@@ -612,10 +642,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ABFB296-438E-1747-ABC9-555CDE54E2A4}">
-  <dimension ref="A2:C14"/>
+  <dimension ref="A2:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -640,32 +670,32 @@
         <v>34</v>
       </c>
       <c r="B3">
-        <v>5000000</v>
+        <v>75000000000</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B4">
         <v>475</v>
       </c>
       <c r="C4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5">
         <v>234</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -676,90 +706,101 @@
         <v>0.9</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B7">
         <v>2.13</v>
       </c>
       <c r="C7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" t="s">
         <v>40</v>
-      </c>
-      <c r="B8" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9">
         <v>250</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B10">
         <v>250</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B11">
         <f>B13-B10</f>
         <v>115</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B12">
         <v>0</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B13" s="2">
         <v>365</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15">
+        <v>0.58799999999999997</v>
+      </c>
+      <c r="C15" t="s">
         <v>66</v>
-      </c>
-      <c r="B14">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -816,7 +857,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -827,7 +868,7 @@
         <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -888,7 +929,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -913,7 +954,7 @@
   <dimension ref="A2:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -926,23 +967,23 @@
         <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3">
         <v>70000</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B4">
         <v>10</v>
@@ -1048,10 +1089,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F27F4F09-9562-8F4C-A40E-927BF5DC3D04}">
-  <dimension ref="A2:C5"/>
+  <dimension ref="A2:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1069,17 +1110,24 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>77</v>
+      </c>
+      <c r="B3">
+        <v>0.18540000000000001</v>
+      </c>
+      <c r="C3" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>49</v>
+        <v>46</v>
+      </c>
+      <c r="B4">
+        <v>1E-3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1089,10 +1137,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C79E67D-1E01-B146-9A1B-D29FD51A6D12}">
-  <dimension ref="A2:B3"/>
+  <dimension ref="A2:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1107,7 +1155,74 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>67</v>
+      </c>
+      <c r="B4">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1119,8 +1234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{635D5B4B-AA0D-8346-A63A-AAC97E12BBE4}">
   <dimension ref="A2:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1154,7 +1269,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -1162,7 +1277,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -1170,7 +1285,10 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>57</v>
+      </c>
+      <c r="B7">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1209,7 +1327,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B3">
         <v>139</v>
@@ -1231,7 +1349,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -1254,7 +1372,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62385A2F-9BCF-E84D-987B-70F09662E5AB}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1290,7 +1410,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -1314,7 +1434,7 @@
   <dimension ref="A2:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:C5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1327,12 +1447,12 @@
         <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B3">
         <v>900</v>
@@ -1348,7 +1468,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1358,10 +1478,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D375DA5D-47B4-034B-A28D-715AAE1B79FC}">
-  <dimension ref="A2:B2"/>
+  <dimension ref="A2:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1374,6 +1494,27 @@
         <v>21</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>74</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1381,12 +1522,44 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20386E3A-C567-1F42-9477-9B986FE1CE0F}">
-  <dimension ref="A1"/>
+  <dimension ref="A2:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
printing outputs looking good
</commit_message>
<xml_diff>
--- a/data/mine_attributes.xlsx
+++ b/data/mine_attributes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/Documents/University Work/summer internship/FUSE/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6074664C-3846-964D-A303-777AC02383A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E9CFD24-1332-CE48-AFA4-E143CFE1228D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="500" windowWidth="21560" windowHeight="17500" xr2:uid="{E883CBF3-2CDB-0D4C-B75C-CDFD4FA8C312}"/>
+    <workbookView xWindow="100" yWindow="500" windowWidth="21560" windowHeight="17500" firstSheet="4" activeTab="11" xr2:uid="{E883CBF3-2CDB-0D4C-B75C-CDFD4FA8C312}"/>
   </bookViews>
   <sheets>
     <sheet name="macro details" sheetId="8" r:id="rId1"/>
@@ -644,7 +644,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ABFB296-438E-1747-ABC9-555CDE54E2A4}">
   <dimension ref="A2:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -953,7 +953,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA6ED9ED-AFC7-5E4D-A019-3E513DE76C3A}">
   <dimension ref="A2:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -975,7 +975,7 @@
         <v>42</v>
       </c>
       <c r="B3">
-        <v>70000</v>
+        <v>7000</v>
       </c>
       <c r="C3" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
finished longwall method moved the mining packages to the longwall or room and pillar method sheets still need to implement the equivelant lift matrix on the afc drives
</commit_message>
<xml_diff>
--- a/data/mine_attributes.xlsx
+++ b/data/mine_attributes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/Documents/University Work/summer work experience/Imperial College/FUSE/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C600275-94D7-DF4A-BF87-1C6ABBADDB75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{790C9465-9AEB-9F4B-8260-55E4ACE49A4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34260" yWindow="-1120" windowWidth="28800" windowHeight="17500" firstSheet="1" activeTab="9" xr2:uid="{E883CBF3-2CDB-0D4C-B75C-CDFD4FA8C312}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" firstSheet="2" activeTab="2" xr2:uid="{E883CBF3-2CDB-0D4C-B75C-CDFD4FA8C312}"/>
   </bookViews>
   <sheets>
     <sheet name="macro details" sheetId="8" r:id="rId1"/>
@@ -28,6 +28,7 @@
     <sheet name="worker" sheetId="9" r:id="rId13"/>
     <sheet name="borer miner" sheetId="17" r:id="rId14"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId15"/>
+    <sheet name="Sheet2" sheetId="19" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="91">
   <si>
     <t xml:space="preserve">company </t>
   </si>
@@ -236,9 +237,6 @@
     <t>non operating</t>
   </si>
   <si>
-    <t>MADEUP</t>
-  </si>
-  <si>
     <t>mining packages</t>
   </si>
   <si>
@@ -284,32 +282,53 @@
     <t>electricity</t>
   </si>
   <si>
+    <t>kWh</t>
+  </si>
+  <si>
+    <t>#taken from continuous miner</t>
+  </si>
+  <si>
+    <t>#educated guess</t>
+  </si>
+  <si>
+    <t># guess as it is an automated proces</t>
+  </si>
+  <si>
+    <t>cost</t>
+  </si>
+  <si>
+    <t>attrition</t>
+  </si>
+  <si>
+    <t>https://www.komatsu.com/en/products/longwall/shearers/7ls5b/</t>
+  </si>
+  <si>
+    <t>drive_power</t>
+  </si>
+  <si>
+    <t>kw/unit</t>
+  </si>
+  <si>
+    <t>WXO3</t>
+  </si>
+  <si>
+    <t>https://www.komatsu.com/en/products/underground-hard-rock-haulage/lhd/wx03/#specifications</t>
+  </si>
+  <si>
+    <t>max output</t>
+  </si>
+  <si>
+    <t>tph</t>
+  </si>
+  <si>
     <t>#guess</t>
-  </si>
-  <si>
-    <t>kWh</t>
-  </si>
-  <si>
-    <t>#taken from continuous miner</t>
-  </si>
-  <si>
-    <t>#educated guess</t>
-  </si>
-  <si>
-    <t># guess as it is an automated proces</t>
-  </si>
-  <si>
-    <t>cost</t>
-  </si>
-  <si>
-    <t>attrition</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -320,6 +339,19 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF1B232A"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF1B232A"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -345,12 +377,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -665,10 +700,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ABFB296-438E-1747-ABC9-555CDE54E2A4}">
-  <dimension ref="A2:C15"/>
+  <dimension ref="A2:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -729,7 +764,7 @@
         <v>0.9</v>
       </c>
       <c r="C6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -809,21 +844,13 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B14">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+        <v>0.58799999999999997</v>
+      </c>
+      <c r="C14" t="s">
         <v>65</v>
-      </c>
-      <c r="B15">
-        <v>0.58799999999999997</v>
-      </c>
-      <c r="C15" t="s">
-        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -834,10 +861,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20386E3A-C567-1F42-9477-9B986FE1CE0F}">
-  <dimension ref="A2:D5"/>
+  <dimension ref="A2:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -855,10 +882,10 @@
         <v>31</v>
       </c>
       <c r="B3">
-        <v>746</v>
+        <v>700</v>
       </c>
       <c r="C3" t="s">
-        <v>79</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -869,7 +896,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -877,7 +904,18 @@
         <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>74</v>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" s="5">
+        <v>6000</v>
+      </c>
+      <c r="C6" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -887,10 +925,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{231CCEC4-3D3D-4143-AE0F-E82354A19379}">
-  <dimension ref="A2:C6"/>
+  <dimension ref="A2:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -898,7 +936,7 @@
     <col min="1" max="1" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -909,29 +947,32 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>24</v>
       </c>
       <c r="B3">
-        <v>10</v>
+        <v>2.722</v>
       </c>
       <c r="C3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>31</v>
       </c>
       <c r="B4">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="C4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -939,12 +980,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -957,7 +998,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:C3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1110,10 +1151,10 @@
         <v>600</v>
       </c>
       <c r="C4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1124,7 +1165,7 @@
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1222,11 +1263,23 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{895B826A-901F-DC4B-809A-B5BB3FCDC7F7}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F27F4F09-9562-8F4C-A40E-927BF5DC3D04}">
   <dimension ref="A2:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -1245,13 +1298,13 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B3">
         <v>0.18540000000000001</v>
       </c>
       <c r="C3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1262,7 +1315,7 @@
         <v>1E-3</v>
       </c>
       <c r="C4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1272,15 +1325,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C79E67D-1E01-B146-9A1B-D29FD51A6D12}">
-  <dimension ref="A2:B11"/>
+  <dimension ref="A2:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -1288,76 +1344,95 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B4">
         <v>131</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B8">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B10">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>55</v>
       </c>
       <c r="B11">
         <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1367,10 +1442,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{635D5B4B-AA0D-8346-A63A-AAC97E12BBE4}">
-  <dimension ref="A2:B7"/>
+  <dimension ref="A2:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A8" sqref="A8:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1424,6 +1499,14 @@
       </c>
       <c r="B7">
         <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -1566,10 +1649,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6659977-9172-CD46-8451-C5DE37D17549}">
-  <dimension ref="A2:D5"/>
+  <dimension ref="A2:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1577,48 +1660,57 @@
     <col min="1" max="1" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>26</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="4" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>49</v>
       </c>
-      <c r="B3">
+      <c r="B4">
         <v>900</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>31</v>
       </c>
-      <c r="B4">
-        <v>1000</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B5">
+        <v>1057</v>
+      </c>
+      <c r="C5" t="s">
         <v>30</v>
       </c>
-      <c r="D4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="D5" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>50</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1628,15 +1720,15 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D375DA5D-47B4-034B-A28D-715AAE1B79FC}">
-  <dimension ref="A2:B5"/>
+  <dimension ref="A2:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -1644,28 +1736,31 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="B3">
-        <v>746</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>84</v>
       </c>
       <c r="B4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1693,7 +1788,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1701,7 +1796,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B4">
         <v>0</v>

</xml_diff>

<commit_message>
adding inits beginning reaction process
</commit_message>
<xml_diff>
--- a/data/mine_attributes.xlsx
+++ b/data/mine_attributes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/Documents/University Work/summer work experience/Imperial College/FUSE/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C4365D7-3636-2349-A1CB-6B491A8B87C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3973F4A-CDF6-6C46-B332-1AD9405810B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" firstSheet="2" activeTab="7" xr2:uid="{E883CBF3-2CDB-0D4C-B75C-CDFD4FA8C312}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" firstSheet="2" activeTab="12" xr2:uid="{E883CBF3-2CDB-0D4C-B75C-CDFD4FA8C312}"/>
   </bookViews>
   <sheets>
     <sheet name="macro details" sheetId="8" r:id="rId1"/>
@@ -1079,8 +1079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA6ED9ED-AFC7-5E4D-A019-3E513DE76C3A}">
   <dimension ref="A2:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1337,7 +1337,7 @@
   <dimension ref="A2:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1454,7 +1454,7 @@
   <dimension ref="A2:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:B8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1731,8 +1731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D375DA5D-47B4-034B-A28D-715AAE1B79FC}">
   <dimension ref="A2:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>